<commit_message>
Just need to deal with null and 0
</commit_message>
<xml_diff>
--- a/Digital_Data.xlsx
+++ b/Digital_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365-my.sharepoint.com/personal/ghadir_siyam_uk_bp_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/rjb255_cam_ac_uk/Documents/University/CUES/Hackathon 2021/bpWindTurbines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{951328F8-FFBD-4B2B-8775-912D745E4BFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{633D6C6F-CDC8-4CBD-86AD-C850048A12C6}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{951328F8-FFBD-4B2B-8775-912D745E4BFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F437A155-3502-4268-AB91-1C3196AF3517}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F03C4418-4E6F-4433-8BAB-911CBF0150FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F03C4418-4E6F-4433-8BAB-911CBF0150FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$67</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water depth </t>
   </si>
   <si>
     <t>a1</t>
@@ -131,12 +128,15 @@
   <si>
     <t>Europe</t>
   </si>
+  <si>
+    <t>Water depth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,10 +515,10 @@
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -534,7 +534,7 @@
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,48 +542,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1085</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2">
         <v>250</v>
@@ -607,24 +607,24 @@
         <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1086</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3">
         <v>250</v>
@@ -648,24 +648,24 @@
         <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1087</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4">
         <v>250</v>
@@ -686,27 +686,27 @@
         <v>21.5</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1088</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
       <c r="D5">
         <v>240</v>
@@ -727,27 +727,27 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1089</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>240</v>
@@ -771,24 +771,24 @@
         <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
         <v>16</v>
       </c>
-      <c r="M6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1090</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>232</v>
@@ -809,24 +809,24 @@
         <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1091</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8">
         <v>225</v>
@@ -844,27 +844,27 @@
         <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s">
         <v>24</v>
       </c>
-      <c r="L8" t="s">
-        <v>25</v>
-      </c>
       <c r="M8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1092</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
       </c>
       <c r="D9">
         <v>225</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9">
         <v>18</v>
@@ -888,24 +888,24 @@
         <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1093</v>
       </c>
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
       <c r="D10">
         <v>220</v>
@@ -926,27 +926,27 @@
         <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1094</v>
       </c>
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -967,27 +967,27 @@
         <v>9.5</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1095</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>190</v>
@@ -999,33 +999,33 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12">
         <v>9.6</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1096</v>
       </c>
       <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
       </c>
       <c r="D13">
         <v>185</v>
@@ -1043,27 +1043,27 @@
         <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1097</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>180</v>
@@ -1075,33 +1075,33 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14">
         <v>14</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1098</v>
       </c>
       <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
         <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
       </c>
       <c r="D15">
         <v>180</v>
@@ -1119,27 +1119,27 @@
         <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1099</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16">
         <v>173</v>
@@ -1151,33 +1151,33 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I16">
         <v>20</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
         <v>24</v>
       </c>
-      <c r="L16" t="s">
-        <v>25</v>
-      </c>
       <c r="M16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1100</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>170</v>
@@ -1189,33 +1189,33 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17">
         <v>20</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" t="s">
         <v>16</v>
       </c>
-      <c r="M17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1101</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18">
         <v>160</v>
@@ -1227,33 +1227,33 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18">
         <v>20</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" t="s">
         <v>16</v>
       </c>
-      <c r="M18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1102</v>
       </c>
       <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
         <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
       </c>
       <c r="D19">
         <v>160</v>
@@ -1277,24 +1277,24 @@
         <v>48</v>
       </c>
       <c r="K19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" t="s">
         <v>16</v>
       </c>
-      <c r="M19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1103</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>157</v>
@@ -1318,24 +1318,24 @@
         <v>55</v>
       </c>
       <c r="K20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20" t="s">
         <v>16</v>
       </c>
-      <c r="M20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1104</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>154</v>
@@ -1359,24 +1359,24 @@
         <v>28</v>
       </c>
       <c r="K21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
         <v>24</v>
       </c>
-      <c r="L21" t="s">
-        <v>25</v>
-      </c>
       <c r="M21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1105</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22">
         <v>150</v>
@@ -1397,27 +1397,27 @@
         <v>14</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" t="s">
         <v>16</v>
       </c>
-      <c r="M22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1106</v>
       </c>
       <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
         <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
       </c>
       <c r="D23">
         <v>150</v>
@@ -1429,30 +1429,30 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1107</v>
       </c>
       <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
         <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
       </c>
       <c r="D24">
         <v>150</v>
@@ -1473,24 +1473,24 @@
         <v>48</v>
       </c>
       <c r="K24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1108</v>
       </c>
       <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
         <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
       </c>
       <c r="D25">
         <v>150</v>
@@ -1508,27 +1508,27 @@
         <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1109</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26">
         <v>150</v>
@@ -1549,24 +1549,24 @@
         <v>36</v>
       </c>
       <c r="K26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1110</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27">
         <v>150</v>
@@ -1584,27 +1584,27 @@
         <v>20</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1111</v>
       </c>
       <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
         <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
       </c>
       <c r="D28">
         <v>150</v>
@@ -1628,24 +1628,24 @@
         <v>26</v>
       </c>
       <c r="K28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1112</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29">
         <v>150</v>
@@ -1669,24 +1669,24 @@
         <v>48</v>
       </c>
       <c r="K29" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" t="s">
         <v>24</v>
       </c>
-      <c r="L29" t="s">
-        <v>25</v>
-      </c>
       <c r="M29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1113</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30">
         <v>140</v>
@@ -1710,24 +1710,24 @@
         <v>48</v>
       </c>
       <c r="K30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" t="s">
         <v>29</v>
       </c>
-      <c r="L30" t="s">
-        <v>16</v>
-      </c>
-      <c r="M30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1114</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31">
         <v>140</v>
@@ -1748,24 +1748,24 @@
         <v>37</v>
       </c>
       <c r="K31" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
         <v>29</v>
       </c>
-      <c r="L31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1115</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D32">
         <v>140</v>
@@ -1789,24 +1789,24 @@
         <v>44</v>
       </c>
       <c r="K32" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" t="s">
         <v>24</v>
       </c>
-      <c r="L32" t="s">
-        <v>25</v>
-      </c>
       <c r="M32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1116</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <v>130</v>
@@ -1830,24 +1830,24 @@
         <v>56</v>
       </c>
       <c r="K33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1117</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34">
         <v>120</v>
@@ -1868,27 +1868,27 @@
         <v>5.6</v>
       </c>
       <c r="J34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K34" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" t="s">
         <v>24</v>
       </c>
-      <c r="L34" t="s">
-        <v>25</v>
-      </c>
       <c r="M34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1118</v>
       </c>
       <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
         <v>13</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
       </c>
       <c r="D35">
         <v>120</v>
@@ -1912,24 +1912,24 @@
         <v>31</v>
       </c>
       <c r="K35" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" t="s">
+        <v>15</v>
+      </c>
+      <c r="M35" t="s">
         <v>29</v>
       </c>
-      <c r="L35" t="s">
-        <v>16</v>
-      </c>
-      <c r="M35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1119</v>
       </c>
       <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
         <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
       </c>
       <c r="D36">
         <v>120</v>
@@ -1953,24 +1953,24 @@
         <v>24</v>
       </c>
       <c r="K36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M36" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1120</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37">
         <v>105</v>
@@ -1991,27 +1991,27 @@
         <v>6.3</v>
       </c>
       <c r="J37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K37" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" t="s">
         <v>24</v>
       </c>
-      <c r="L37" t="s">
-        <v>25</v>
-      </c>
       <c r="M37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1121</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38">
         <v>100</v>
@@ -2032,27 +2032,27 @@
         <v>16</v>
       </c>
       <c r="J38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1122</v>
       </c>
       <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
         <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
       </c>
       <c r="D39">
         <v>100</v>
@@ -2076,24 +2076,24 @@
         <v>32</v>
       </c>
       <c r="K39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1123</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40">
         <v>100</v>
@@ -2111,27 +2111,27 @@
         <v>9</v>
       </c>
       <c r="J40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K40" t="s">
+        <v>23</v>
+      </c>
+      <c r="L40" t="s">
         <v>24</v>
       </c>
-      <c r="L40" t="s">
-        <v>25</v>
-      </c>
       <c r="M40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1124</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41">
         <v>100</v>
@@ -2152,27 +2152,27 @@
         <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" t="s">
         <v>29</v>
       </c>
-      <c r="L41" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1125</v>
       </c>
       <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
         <v>13</v>
-      </c>
-      <c r="C42" t="s">
-        <v>14</v>
       </c>
       <c r="D42">
         <v>100</v>
@@ -2196,24 +2196,24 @@
         <v>32</v>
       </c>
       <c r="K42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>1126</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>100</v>
@@ -2237,24 +2237,24 @@
         <v>30</v>
       </c>
       <c r="K43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>1127</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D44">
         <v>100</v>
@@ -2278,24 +2278,24 @@
         <v>36</v>
       </c>
       <c r="K44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>1128</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45">
         <v>96</v>
@@ -2307,33 +2307,33 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I45">
         <v>8.5</v>
       </c>
       <c r="J45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1129</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46">
         <v>90</v>
@@ -2354,24 +2354,24 @@
         <v>22</v>
       </c>
       <c r="K46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1130</v>
       </c>
       <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
         <v>13</v>
-      </c>
-      <c r="C47" t="s">
-        <v>14</v>
       </c>
       <c r="D47">
         <v>90</v>
@@ -2383,33 +2383,33 @@
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I47">
         <v>17</v>
       </c>
       <c r="J47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1131</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D48">
         <v>89</v>
@@ -2421,33 +2421,33 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I48">
         <v>5</v>
       </c>
       <c r="J48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K48" t="s">
+        <v>23</v>
+      </c>
+      <c r="L48" t="s">
         <v>24</v>
       </c>
-      <c r="L48" t="s">
-        <v>25</v>
-      </c>
       <c r="M48" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1132</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D49">
         <v>85</v>
@@ -2468,27 +2468,27 @@
         <v>5.4</v>
       </c>
       <c r="J49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K49" t="s">
+        <v>23</v>
+      </c>
+      <c r="L49" t="s">
         <v>24</v>
       </c>
-      <c r="L49" t="s">
-        <v>25</v>
-      </c>
       <c r="M49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1133</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D50">
         <v>85</v>
@@ -2512,24 +2512,24 @@
         <v>60</v>
       </c>
       <c r="K50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1134</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D51">
         <v>80</v>
@@ -2541,33 +2541,33 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I51">
         <v>10</v>
       </c>
       <c r="J51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M51" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1135</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D52">
         <v>80</v>
@@ -2582,33 +2582,33 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I52">
         <v>25</v>
       </c>
       <c r="J52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M52" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1136</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D53">
         <v>80</v>
@@ -2620,33 +2620,33 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I53">
         <v>10.35</v>
       </c>
       <c r="J53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M53" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1137</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D54">
         <v>80</v>
@@ -2670,24 +2670,24 @@
         <v>27</v>
       </c>
       <c r="K54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M54" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>1138</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55">
         <v>76</v>
@@ -2705,27 +2705,27 @@
         <v>25</v>
       </c>
       <c r="J55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K55" t="s">
+        <v>23</v>
+      </c>
+      <c r="L55" t="s">
         <v>24</v>
       </c>
-      <c r="L55" t="s">
-        <v>25</v>
-      </c>
       <c r="M55" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1139</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D56">
         <v>70</v>
@@ -2749,24 +2749,24 @@
         <v>12</v>
       </c>
       <c r="K56" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" t="s">
         <v>24</v>
       </c>
-      <c r="L56" t="s">
-        <v>25</v>
-      </c>
       <c r="M56" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1140</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57">
         <v>70</v>
@@ -2787,27 +2787,27 @@
         <v>5</v>
       </c>
       <c r="J57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>1141</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D58">
         <v>70</v>
@@ -2828,27 +2828,27 @@
         <v>30</v>
       </c>
       <c r="J58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>1142</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D59">
         <v>63</v>
@@ -2863,33 +2863,33 @@
         <v>180</v>
       </c>
       <c r="H59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I59">
         <v>6.2</v>
       </c>
       <c r="J59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M59" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>1143</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D60">
         <v>60</v>
@@ -2904,33 +2904,33 @@
         <v>150</v>
       </c>
       <c r="H60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I60">
         <v>8.4499999999999993</v>
       </c>
       <c r="J60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M60" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>1144</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D61">
         <v>60</v>
@@ -2954,24 +2954,24 @@
         <v>24</v>
       </c>
       <c r="K61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M61" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>1145</v>
       </c>
       <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" t="s">
         <v>13</v>
-      </c>
-      <c r="C62" t="s">
-        <v>14</v>
       </c>
       <c r="D62">
         <v>60</v>
@@ -2992,27 +2992,27 @@
         <v>13</v>
       </c>
       <c r="J62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M62" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>1146</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D63">
         <v>57</v>
@@ -3027,33 +3027,33 @@
         <v>90</v>
       </c>
       <c r="H63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I63">
         <v>4.7</v>
       </c>
       <c r="J63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K63" t="s">
+        <v>28</v>
+      </c>
+      <c r="L63" t="s">
+        <v>24</v>
+      </c>
+      <c r="M63" t="s">
         <v>29</v>
       </c>
-      <c r="L63" t="s">
-        <v>25</v>
-      </c>
-      <c r="M63" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>1147</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D64">
         <v>45</v>
@@ -3074,27 +3074,27 @@
         <v>5.6</v>
       </c>
       <c r="J64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K64" t="s">
+        <v>28</v>
+      </c>
+      <c r="L64" t="s">
+        <v>15</v>
+      </c>
+      <c r="M64" t="s">
         <v>29</v>
       </c>
-      <c r="L64" t="s">
-        <v>16</v>
-      </c>
-      <c r="M64" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>1148</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D65">
         <v>45</v>
@@ -3115,27 +3115,27 @@
         <v>5.6</v>
       </c>
       <c r="J65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K65" t="s">
+        <v>28</v>
+      </c>
+      <c r="L65" t="s">
+        <v>24</v>
+      </c>
+      <c r="M65" t="s">
         <v>29</v>
       </c>
-      <c r="L65" t="s">
-        <v>25</v>
-      </c>
-      <c r="M65" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>1149</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66">
         <v>40</v>
@@ -3156,27 +3156,27 @@
         <v>25</v>
       </c>
       <c r="J66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>1150</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D67">
         <v>30</v>
@@ -3197,16 +3197,16 @@
         <v>15</v>
       </c>
       <c r="J67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K67" t="s">
+        <v>28</v>
+      </c>
+      <c r="L67" t="s">
+        <v>15</v>
+      </c>
+      <c r="M67" t="s">
         <v>29</v>
-      </c>
-      <c r="L67" t="s">
-        <v>16</v>
-      </c>
-      <c r="M67" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3225,6 +3225,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064E3E7C126BE4540B20C050CEB86B435" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="234474e708f24905dcb7b6cc8481db02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67123090-1f18-410c-a08b-b268c47f9cd3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6d9885766c01766e494b22684b2d23d" ns2:_="">
     <xsd:import namespace="67123090-1f18-410c-a08b-b268c47f9cd3"/>
@@ -3356,20 +3362,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303F99FB-BD7D-4035-8492-11BB66CC96A8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303F99FB-BD7D-4035-8492-11BB66CC96A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BE92EF1-279C-464B-9EE1-E7263DE2FAB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54FCC43A-0DF9-4985-AD62-FAF26FE274B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54FCC43A-0DF9-4985-AD62-FAF26FE274B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BE92EF1-279C-464B-9EE1-E7263DE2FAB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="67123090-1f18-410c-a08b-b268c47f9cd3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>